<commit_message>
added stuff to the api
</commit_message>
<xml_diff>
--- a/Planing/api.xlsx
+++ b/Planing/api.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Projekts/Virtual Shop/Planing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1DBD22-D4A7-7D46-AB71-DA2F8CFF77C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A6F650-02C3-3C43-A044-3A5F79EACC22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EA3522A4-B874-ED44-BC4B-D8C3226EC949}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{EA3522A4-B874-ED44-BC4B-D8C3226EC949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Pfad</t>
   </si>
@@ -114,9 +114,6 @@
     <t>UserName, Password</t>
   </si>
   <si>
-    <t>SecurityCookie, DATA</t>
-  </si>
-  <si>
     <t>API</t>
   </si>
   <si>
@@ -124,6 +121,27 @@
   </si>
   <si>
     <t>main</t>
+  </si>
+  <si>
+    <t>/review</t>
+  </si>
+  <si>
+    <t>adds a new Review</t>
+  </si>
+  <si>
+    <t>SecurityCookie, Product, Review</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>SecurityCookie, Product</t>
   </si>
 </sst>
 </file>
@@ -184,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -192,14 +210,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -305,6 +324,24 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -319,14 +356,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61F0A0EE-5E26-9840-8282-A5A0D53D7C4D}" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:E9" xr:uid="{2ED6B817-35D0-9B45-A9CA-AC8DB08AB91B}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61F0A0EE-5E26-9840-8282-A5A0D53D7C4D}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:F10" xr:uid="{2ED6B817-35D0-9B45-A9CA-AC8DB08AB91B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E5D14F5B-69B7-A24D-BDE9-1E01AAF77D67}" name="API"/>
-    <tableColumn id="2" xr3:uid="{48F144B3-0CE2-5448-98E6-52F961859CC0}" name="Pfad" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{52CD4DA6-C319-2E47-860F-C7FB33CD615A}" name="Name" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{22F3EAA9-5EC1-0543-8DF9-36ACAE6B2D8A}" name="Function" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{C1C354E4-C567-8747-B535-2D8032E56242}" name="Body" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{48F144B3-0CE2-5448-98E6-52F961859CC0}" name="Pfad" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{52CD4DA6-C319-2E47-860F-C7FB33CD615A}" name="Name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{22F3EAA9-5EC1-0543-8DF9-36ACAE6B2D8A}" name="Function" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C1C354E4-C567-8747-B535-2D8032E56242}" name="Body" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{26A20DC2-574F-8B49-B217-46C0B60A5C16}" name="request" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -629,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEF0AB3-214A-794D-88AB-70349991E968}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,12 +678,12 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="61.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -659,10 +697,13 @@
       <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -676,10 +717,11 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
@@ -693,10 +735,11 @@
       <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -710,10 +753,11 @@
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>21</v>
@@ -725,10 +769,13 @@
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>22</v>
@@ -740,10 +787,13 @@
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -755,10 +805,13 @@
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>24</v>
@@ -768,12 +821,15 @@
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>24</v>
@@ -783,7 +839,28 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found the bugs, fixed the bugs
found a new Bug
</commit_message>
<xml_diff>
--- a/Planing/api.xlsx
+++ b/Planing/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Projekts/Virtual Shop/Planing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B304CF2-9C8E-9D4A-8D54-0055F06C3F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3FBA50-3BE5-024D-B209-409711DEACCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EA3522A4-B874-ED44-BC4B-D8C3226EC949}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Pfad</t>
   </si>
@@ -138,9 +138,6 @@
     <t>get</t>
   </si>
   <si>
-    <t>put</t>
-  </si>
-  <si>
     <t>SecurityCookie, Product</t>
   </si>
   <si>
@@ -157,6 +154,24 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Webpage</t>
+  </si>
+  <si>
+    <t>managerpage</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>POST</t>
   </si>
 </sst>
 </file>
@@ -701,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEF0AB3-214A-794D-88AB-70349991E968}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +751,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -755,7 +770,9 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -774,7 +791,9 @@
       <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -793,7 +812,9 @@
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -865,13 +886,13 @@
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -886,10 +907,10 @@
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -917,23 +938,67 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>8081</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a lot of stuff
- fixed bug
- started watson api dev
- more querys
- more stuff
</commit_message>
<xml_diff>
--- a/Planing/api.xlsx
+++ b/Planing/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Projekts/Virtual Shop/Planing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3FBA50-3BE5-024D-B209-409711DEACCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D585986-BB32-3D4F-A2C7-74AC334AA9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EA3522A4-B874-ED44-BC4B-D8C3226EC949}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{EA3522A4-B874-ED44-BC4B-D8C3226EC949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>Pfad</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
   </si>
 </sst>
 </file>
@@ -719,7 +722,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,7 +835,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -997,6 +1000,12 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
       <c r="C18">
         <v>5000</v>
       </c>

</xml_diff>